<commit_message>
Subida de archivo 100000.xlsx
</commit_message>
<xml_diff>
--- a/100000.xlsx
+++ b/100000.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,170 +436,200 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>FILTRO</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>M-COD</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>PRODUCTO</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>DETALLES</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>STOCK</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>DISTRIB</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>FOTO</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>NOTEBOOK</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
         <v>414308</v>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="C2" t="inlineStr">
         <is>
           <t xml:space="preserve"> NB AS 16 I5-12 16 512 FREE</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>Notebook ASUS X1605ZA-MB292 16.0" WUXGA LED IPS, Core i5-12500H hasta 4.5GHz, 16GB DD</t>
         </is>
       </c>
-      <c r="D2" t="n">
+      <c r="E2" t="n">
         <v>20</v>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>S/. 2,662</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>https://www.deltron.com.pe/modulos/productos/items/image_ext.php?item=NBASX1605ZMB2</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>NOTEBOOK</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
         <v>442279</v>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="C3" t="inlineStr">
         <is>
           <t xml:space="preserve"> NB LEN V15 CI5/16GB/512G/W11P</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>Notebook Lenovo V15 G4 IRU, 15.6" LCD LED FHD, Core i5-1335U 1.3/4.6GHz, 16GB DDR4-32</t>
         </is>
       </c>
-      <c r="D3" t="n">
+      <c r="E3" t="n">
         <v>20</v>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>S/. 3,018</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="G3" t="inlineStr">
         <is>
           <t>https://www.deltron.com.pe/modulos/productos/items/image_ext.php?item=NBLEN83CCS00400</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>NOTEBOOK</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
         <v>441124</v>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="C4" t="inlineStr">
         <is>
           <t xml:space="preserve"> NB LEN V15 I7-1355U/16/512/FRE</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>Notebook Lenovo V15 G4 IRU, 15.6" FHD TN, Core i7-1355U 1.7 / 5.0GHz, 16GB DDR4-3200M</t>
         </is>
       </c>
-      <c r="D4" t="n">
+      <c r="E4" t="n">
         <v>20</v>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="F4" t="inlineStr">
         <is>
           <t>S/. 3,273</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="G4" t="inlineStr">
         <is>
           <t>https://www.deltron.com.pe/modulos/productos/items/image_ext.php?item=NBLEN83A100ERLM</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>NOTEBOOK</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
         <v>440989</v>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
           <t xml:space="preserve"> NB LEN V15 I7-1355U/16/1SS/FRE</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="D5" t="inlineStr">
         <is>
           <t>Notebook Lenovo V15 G4 IRU,15.6" FHD TN, Core i7-1355U hasta 5.0GHz,16GB DDR4-3200MHz</t>
         </is>
       </c>
-      <c r="D5" t="n">
+      <c r="E5" t="n">
         <v>1</v>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t>S/. 3,467</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="G5" t="inlineStr">
         <is>
           <t>https://www.deltron.com.pe/modulos/productos/items/image_ext.php?item=NBLEN83A100ESLM</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>NOTEBOOK</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
         <v>414307</v>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="C6" t="inlineStr">
         <is>
           <t xml:space="preserve"> NB AS 16 I9-13 16 1TB FREE</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="D6" t="inlineStr">
         <is>
           <t>Notebook ASUS X1605VA-MB195 16.0" WUXGA LED IPS, Core i9-13900H hasta 5.4GHz, 16GB DD</t>
         </is>
       </c>
-      <c r="D6" t="n">
+      <c r="E6" t="n">
         <v>9</v>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="F6" t="inlineStr">
         <is>
           <t>S/. 3,952</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="G6" t="inlineStr">
         <is>
           <t>https://www.deltron.com.pe/modulos/productos/items/image_ext.php?item=NBASX1605MB195</t>
         </is>

</xml_diff>